<commit_message>
commit for final report
</commit_message>
<xml_diff>
--- a/5th_report/cmpaund_result.xlsx
+++ b/5th_report/cmpaund_result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\lecture2019\winter\complex_network\5th_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C6255F-4DFB-430C-8B8B-6172F4F09F7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4357358F-9ADE-4265-B95F-6EC68BBB4954}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1820" yWindow="1820" windowWidth="16510" windowHeight="8910" xr2:uid="{9D07478E-DF48-483E-AA34-264D1FEF8655}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{9D07478E-DF48-483E-AA34-264D1FEF8655}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>small network</t>
     <phoneticPr fontId="1"/>
@@ -83,6 +83,10 @@
   </si>
   <si>
     <t>(5,6)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>＊</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -115,12 +119,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -129,9 +148,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -450,7 +475,7 @@
   <dimension ref="B2:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -462,47 +487,57 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C2" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>1.5</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2.9</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>0.5</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.13600000000000001</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>7</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>